<commit_message>
hint equip dev chance
Signed-off-by: ibicdlcod <504161487@qq.com>
</commit_message>
<xml_diff>
--- a/doc/equip/Equip.xlsx
+++ b/doc/equip/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GuoMuoRuoProject\doc\equip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D61495-0C09-4B91-9D75-EDA4399E3B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2297F4-61B0-4168-8443-FCAA119A02C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2607,16 +2607,41 @@
   <dimension ref="A1:AE583"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C530" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="H541" sqref="H541"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.06640625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="67" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" customWidth="1"/>
+    <col min="1" max="1" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.06640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
@@ -24068,6 +24093,9 @@
         <v>1948</v>
       </c>
       <c r="F541">
+        <v>374</v>
+      </c>
+      <c r="H541">
         <v>374</v>
       </c>
       <c r="I541">

</xml_diff>

<commit_message>
server user ship database
Signed-off-by: ibicdlcod <504161487@qq.com>
</commit_message>
<xml_diff>
--- a/doc/equip/Equip.xlsx
+++ b/doc/equip/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GuoMuoRuoProject\doc\equip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5435377-A876-4A3A-A6BC-118F08853F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9060A9A2-07CB-40FD-8F3C-982DA9BB4B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2528,10 +2528,10 @@
   <dimension ref="A1:AE583"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.06640625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>

</xml_diff>